<commit_message>
Updated stat.xlsx to use partition 2
</commit_message>
<xml_diff>
--- a/rfcyscore/stat.xlsx
+++ b/rfcyscore/stat.xlsx
@@ -824,16 +824,16 @@
         <v>247</v>
       </c>
       <c r="C2" s="4">
-        <v>1.81</v>
+        <v>1.75</v>
       </c>
       <c r="D2" s="4">
-        <v>1.7</v>
+        <v>1.63</v>
       </c>
       <c r="E2" s="5">
-        <v>0.52400000000000002</v>
+        <v>0.57899999999999996</v>
       </c>
       <c r="F2" s="5">
-        <v>0.52500000000000002</v>
+        <v>0.59199999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -844,16 +844,16 @@
         <v>592</v>
       </c>
       <c r="C3" s="4">
-        <v>1.69</v>
+        <v>1.62</v>
       </c>
       <c r="D3" s="4">
-        <v>1.7</v>
+        <v>1.62</v>
       </c>
       <c r="E3" s="5">
-        <v>0.53100000000000003</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="F3" s="5">
-        <v>0.53</v>
+        <v>0.59799999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -864,16 +864,16 @@
         <v>1184</v>
       </c>
       <c r="C4" s="4">
-        <v>1.69</v>
+        <v>1.62</v>
       </c>
       <c r="D4" s="4">
-        <v>1.7</v>
+        <v>1.62</v>
       </c>
       <c r="E4" s="5">
-        <v>0.53100000000000003</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="F4" s="5">
-        <v>0.52900000000000003</v>
+        <v>0.59799999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -884,16 +884,16 @@
         <v>1776</v>
       </c>
       <c r="C5" s="4">
-        <v>1.7</v>
+        <v>1.61</v>
       </c>
       <c r="D5" s="4">
-        <v>1.7</v>
+        <v>1.61</v>
       </c>
       <c r="E5" s="5">
-        <v>0.53</v>
+        <v>0.59</v>
       </c>
       <c r="F5" s="5">
-        <v>0.52800000000000002</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -904,16 +904,16 @@
         <v>2367</v>
       </c>
       <c r="C6" s="4">
-        <v>1.69</v>
+        <v>1.62</v>
       </c>
       <c r="D6" s="4">
-        <v>1.7</v>
+        <v>1.62</v>
       </c>
       <c r="E6" s="5">
-        <v>0.53100000000000003</v>
+        <v>0.58899999999999997</v>
       </c>
       <c r="F6" s="5">
-        <v>0.52900000000000003</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -924,16 +924,16 @@
         <v>592</v>
       </c>
       <c r="C7" s="4">
-        <v>1.71</v>
+        <v>1.59</v>
       </c>
       <c r="D7" s="4">
-        <v>1.71</v>
+        <v>1.59</v>
       </c>
       <c r="E7" s="5">
-        <v>0.51800000000000002</v>
+        <v>0.60899999999999999</v>
       </c>
       <c r="F7" s="5">
-        <v>0.51</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -944,16 +944,16 @@
         <v>1184</v>
       </c>
       <c r="C8" s="4">
-        <v>1.67</v>
+        <v>1.56</v>
       </c>
       <c r="D8" s="4">
-        <v>1.66</v>
+        <v>1.55</v>
       </c>
       <c r="E8" s="5">
-        <v>0.55500000000000005</v>
+        <v>0.629</v>
       </c>
       <c r="F8" s="5">
-        <v>0.54100000000000004</v>
+        <v>0.61899999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -964,16 +964,16 @@
         <v>1776</v>
       </c>
       <c r="C9" s="4">
-        <v>1.66</v>
+        <v>1.54</v>
       </c>
       <c r="D9" s="4">
-        <v>1.66</v>
+        <v>1.53</v>
       </c>
       <c r="E9" s="5">
-        <v>0.55600000000000005</v>
+        <v>0.64200000000000002</v>
       </c>
       <c r="F9" s="5">
-        <v>0.54</v>
+        <v>0.628</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -984,16 +984,16 @@
         <v>2367</v>
       </c>
       <c r="C10" s="4">
-        <v>1.66</v>
+        <v>1.51</v>
       </c>
       <c r="D10" s="4">
-        <v>1.66</v>
+        <v>1.51</v>
       </c>
       <c r="E10" s="5">
-        <v>0.56100000000000005</v>
+        <v>0.65700000000000003</v>
       </c>
       <c r="F10" s="5">
-        <v>0.54500000000000004</v>
+        <v>0.64100000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1004,16 +1004,16 @@
         <v>592</v>
       </c>
       <c r="C11" s="4">
-        <v>1.56</v>
+        <v>1.49</v>
       </c>
       <c r="D11" s="4">
-        <v>1.56</v>
+        <v>1.49</v>
       </c>
       <c r="E11" s="5">
-        <v>0.627</v>
+        <v>0.66900000000000004</v>
       </c>
       <c r="F11" s="5">
-        <v>0.622</v>
+        <v>0.66300000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1024,16 +1024,16 @@
         <v>1184</v>
       </c>
       <c r="C12" s="4">
-        <v>1.5</v>
+        <v>1.43</v>
       </c>
       <c r="D12" s="4">
-        <v>1.5</v>
+        <v>1.42</v>
       </c>
       <c r="E12" s="5">
-        <v>0.66100000000000003</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="F12" s="5">
-        <v>0.65700000000000003</v>
+        <v>0.69799999999999995</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1044,16 +1044,16 @@
         <v>1776</v>
       </c>
       <c r="C13" s="4">
-        <v>1.5</v>
+        <v>1.41</v>
       </c>
       <c r="D13" s="4">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="E13" s="5">
-        <v>0.66200000000000003</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="F13" s="5">
-        <v>0.65600000000000003</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1064,16 +1064,16 @@
         <v>2367</v>
       </c>
       <c r="C14" s="4">
-        <v>1.49</v>
+        <v>1.38</v>
       </c>
       <c r="D14" s="4">
-        <v>1.49</v>
+        <v>1.37</v>
       </c>
       <c r="E14" s="5">
-        <v>0.66800000000000004</v>
+        <v>0.73</v>
       </c>
       <c r="F14" s="5">
-        <v>0.66500000000000004</v>
+        <v>0.72499999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1084,16 +1084,16 @@
         <v>592</v>
       </c>
       <c r="C15" s="4">
-        <v>1.53</v>
+        <v>1.42</v>
       </c>
       <c r="D15" s="4">
-        <v>1.53</v>
+        <v>1.41</v>
       </c>
       <c r="E15" s="5">
-        <v>0.64300000000000002</v>
+        <v>0.71</v>
       </c>
       <c r="F15" s="5">
-        <v>0.64500000000000002</v>
+        <v>0.70699999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1104,16 +1104,16 @@
         <v>1184</v>
       </c>
       <c r="C16" s="4">
-        <v>1.47</v>
+        <v>1.36</v>
       </c>
       <c r="D16" s="4">
-        <v>1.47</v>
+        <v>1.35</v>
       </c>
       <c r="E16" s="5">
-        <v>0.67900000000000005</v>
+        <v>0.73699999999999999</v>
       </c>
       <c r="F16" s="5">
-        <v>0.68100000000000005</v>
+        <v>0.73899999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1124,16 +1124,16 @@
         <v>1776</v>
       </c>
       <c r="C17" s="4">
-        <v>1.43</v>
+        <v>1.32</v>
       </c>
       <c r="D17" s="4">
-        <v>1.43</v>
+        <v>1.31</v>
       </c>
       <c r="E17" s="5">
-        <v>0.69799999999999995</v>
+        <v>0.755</v>
       </c>
       <c r="F17" s="5">
-        <v>0.69699999999999995</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1144,16 +1144,16 @@
         <v>2367</v>
       </c>
       <c r="C18" s="4">
-        <v>1.41</v>
+        <v>1.3</v>
       </c>
       <c r="D18" s="4">
-        <v>1.41</v>
+        <v>1.29</v>
       </c>
       <c r="E18" s="5">
-        <v>0.71099999999999997</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="F18" s="5">
-        <v>0.70899999999999996</v>
+        <v>0.76600000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a new tab LCOCV on PDBbind v2009 (flat)
</commit_message>
<xml_diff>
--- a/rfcyscore/stat.xlsx
+++ b/rfcyscore/stat.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="PDBbind v2007 benchmark (N=195)" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="PDBbind v2013 benchmark (N=592)" sheetId="3" r:id="rId3"/>
     <sheet name="5-fold CV on PDBbind v2013" sheetId="4" r:id="rId4"/>
     <sheet name="LCOCV on PDBbind v2009" sheetId="6" r:id="rId5"/>
+    <sheet name="LCOCV on PDBbind v2009 (flat)" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="100">
   <si>
     <t>model</t>
   </si>
@@ -145,6 +146,189 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biological target </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cluster </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> N </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RMSE </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SD </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rp </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rs </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIV protease                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A </t>
+  </si>
+  <si>
+    <t xml:space="preserve">trypsin                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B </t>
+  </si>
+  <si>
+    <t xml:space="preserve">carbonic anhydrase             </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C </t>
+  </si>
+  <si>
+    <t xml:space="preserve">thrombin                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> D </t>
+  </si>
+  <si>
+    <t xml:space="preserve">protein tyrosine phosphatase   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> E </t>
+  </si>
+  <si>
+    <t xml:space="preserve">factor Xa                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F </t>
+  </si>
+  <si>
+    <t xml:space="preserve">urokinase                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> G </t>
+  </si>
+  <si>
+    <t xml:space="preserve">different similar transporters </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H </t>
+  </si>
+  <si>
+    <t xml:space="preserve">c-AMP dependent kinase         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I </t>
+  </si>
+  <si>
+    <t xml:space="preserve">$\beta$-glucosidase            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> J </t>
+  </si>
+  <si>
+    <t xml:space="preserve">antibodies                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> K </t>
+  </si>
+  <si>
+    <t xml:space="preserve">casein kinase II               </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> L </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ribonuclease                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> M </t>
+  </si>
+  <si>
+    <t xml:space="preserve">thermolysine                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDK2 kinase                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> O </t>
+  </si>
+  <si>
+    <t xml:space="preserve">glutamate receptor 2           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P38 kinase                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Q </t>
+  </si>
+  <si>
+    <t xml:space="preserve">$\beta$-secretase I            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> R </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tRNA-guanine transglycosylase  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> S </t>
+  </si>
+  <si>
+    <t xml:space="preserve">endothiapepsin                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> T </t>
+  </si>
+  <si>
+    <t xml:space="preserve">$\alpha$-mannosidase 2         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> U </t>
+  </si>
+  <si>
+    <t xml:space="preserve">carboxypeptidase A             </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> V </t>
+  </si>
+  <si>
+    <t xml:space="preserve">penicillopepsin                </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> W </t>
+  </si>
+  <si>
+    <t xml:space="preserve">clusters with 4-9 complexes    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> X </t>
+  </si>
+  <si>
+    <t xml:space="preserve">clusters with 2-3 complexes    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Y </t>
+  </si>
+  <si>
+    <t xml:space="preserve">singletons                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Z </t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>standard deviation</t>
   </si>
 </sst>
 </file>
@@ -154,10 +338,23 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -183,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -196,6 +393,19 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4672,4 +4882,2149 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1">
+        <v>188</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1.65</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.53</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0.216</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="J3" s="7">
+        <v>1.51</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0.31</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1.76</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1.56</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0.182</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0.105</v>
+      </c>
+      <c r="R3" s="5">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="S3" s="2">
+        <v>1.77</v>
+      </c>
+      <c r="T3" s="2">
+        <v>1.56</v>
+      </c>
+      <c r="U3" s="3">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="V3" s="3">
+        <v>0.129</v>
+      </c>
+      <c r="W3" s="5">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1">
+        <v>74</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.24</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="S4" s="7">
+        <v>0.93</v>
+      </c>
+      <c r="T4" s="7">
+        <v>0.93</v>
+      </c>
+      <c r="U4" s="8">
+        <v>0.751</v>
+      </c>
+      <c r="V4" s="8">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="W4" s="10">
+        <v>0.53300000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="1">
+        <v>57</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1.35</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2.44</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1.43</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0.161</v>
+      </c>
+      <c r="N5" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="O5" s="2">
+        <v>1.37</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>0.372</v>
+      </c>
+      <c r="R5" s="10">
+        <v>0.27</v>
+      </c>
+      <c r="S5" s="7">
+        <v>2.33</v>
+      </c>
+      <c r="T5" s="7">
+        <v>1.35</v>
+      </c>
+      <c r="U5" s="8">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="W5" s="5">
+        <v>0.17699999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="1">
+        <v>53</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.52</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.505</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1.44</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.68</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="N6" s="2">
+        <v>1.47</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1.45</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="R6" s="10">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="S6" s="7">
+        <v>1.46</v>
+      </c>
+      <c r="T6" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="U6" s="9">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="V6" s="8">
+        <v>0.68</v>
+      </c>
+      <c r="W6" s="5">
+        <v>0.49299999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="1">
+        <v>32</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1.23</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.06</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.313</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0.184</v>
+      </c>
+      <c r="N7" s="2">
+        <v>1.36</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="P7" s="3">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="R7" s="5">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="S7" s="7">
+        <v>1.23</v>
+      </c>
+      <c r="T7" s="7">
+        <v>0.89</v>
+      </c>
+      <c r="U7" s="8">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="V7" s="8">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="W7" s="10">
+        <v>0.45800000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="1">
+        <v>32</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1.18</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0.253</v>
+      </c>
+      <c r="N8" s="2">
+        <v>1.53</v>
+      </c>
+      <c r="O8" s="2">
+        <v>1.02</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0.498</v>
+      </c>
+      <c r="R8" s="5">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="S8" s="2">
+        <v>1.61</v>
+      </c>
+      <c r="T8" s="2">
+        <v>1.07</v>
+      </c>
+      <c r="U8" s="3">
+        <v>0.47</v>
+      </c>
+      <c r="V8" s="3">
+        <v>0.47</v>
+      </c>
+      <c r="W8" s="5">
+        <v>0.33700000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="1">
+        <v>29</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="L9" s="8">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="M9" s="10">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="N9" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="O9" s="2">
+        <v>1.27</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>0.436</v>
+      </c>
+      <c r="R9" s="5">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="S9" s="7">
+        <v>1.05</v>
+      </c>
+      <c r="T9" s="7">
+        <v>1.06</v>
+      </c>
+      <c r="U9" s="8">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="V9" s="3">
+        <v>0.624</v>
+      </c>
+      <c r="W9" s="5">
+        <v>0.441</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="1">
+        <v>29</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0.122</v>
+      </c>
+      <c r="H10" s="5">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1.27</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="K10" s="3">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="L10" s="3">
+        <v>-0.04</v>
+      </c>
+      <c r="M10" s="5">
+        <v>-3.2000000000000001E-2</v>
+      </c>
+      <c r="N10" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0.188</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="R10" s="5">
+        <v>6.2E-2</v>
+      </c>
+      <c r="S10" s="2">
+        <v>1.01</v>
+      </c>
+      <c r="T10" s="7">
+        <v>0.93</v>
+      </c>
+      <c r="U10" s="8">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="V10" s="8">
+        <v>0.123</v>
+      </c>
+      <c r="W10" s="10">
+        <v>9.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="1">
+        <v>17</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.32</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="N11" s="7">
+        <v>0.94</v>
+      </c>
+      <c r="O11" s="7">
+        <v>0.91</v>
+      </c>
+      <c r="P11" s="8">
+        <v>0.748</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="R11" s="10">
+        <v>0.504</v>
+      </c>
+      <c r="S11" s="2">
+        <v>1.06</v>
+      </c>
+      <c r="T11" s="7">
+        <v>0.91</v>
+      </c>
+      <c r="U11" s="9">
+        <v>0.747</v>
+      </c>
+      <c r="V11" s="3">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="W11" s="5">
+        <v>0.46500000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="1">
+        <v>17</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.03</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.316</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.76</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="M12" s="5">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="N12" s="7">
+        <v>0.92</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0.72</v>
+      </c>
+      <c r="P12" s="3">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>0.443</v>
+      </c>
+      <c r="R12" s="5">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="S12" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="T12" s="7">
+        <v>0.68</v>
+      </c>
+      <c r="U12" s="8">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="V12" s="8">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="W12" s="10">
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="1">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1.41</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.43</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1.67</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1.76</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="M13" s="5">
+        <v>0.312</v>
+      </c>
+      <c r="N13" s="2">
+        <v>1.47</v>
+      </c>
+      <c r="O13" s="2">
+        <v>1.51</v>
+      </c>
+      <c r="P13" s="3">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="R13" s="5">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="S13" s="7">
+        <v>1.36</v>
+      </c>
+      <c r="T13" s="7">
+        <v>1.33</v>
+      </c>
+      <c r="U13" s="8">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="V13" s="8">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="W13" s="10">
+        <v>0.61599999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="1">
+        <v>16</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0.254</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.76</v>
+      </c>
+      <c r="J14" s="7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K14" s="9">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="P14" s="3">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="R14" s="5">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="T14" s="2">
+        <v>0.61</v>
+      </c>
+      <c r="U14" s="3">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="V14" s="3">
+        <v>0.309</v>
+      </c>
+      <c r="W14" s="5">
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="1">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.34</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="I15" s="7">
+        <v>1.07</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1.06</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0.505</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="M15" s="5">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="O15" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="P15" s="8">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="R15" s="5">
+        <v>0.371</v>
+      </c>
+      <c r="S15" s="2">
+        <v>1.23</v>
+      </c>
+      <c r="T15" s="2">
+        <v>1.03</v>
+      </c>
+      <c r="U15" s="3">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="V15" s="8">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="W15" s="10">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1">
+        <v>14</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.68</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="J16" s="7">
+        <v>1.03</v>
+      </c>
+      <c r="K16" s="8">
+        <v>0.748</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="M16" s="10">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="N16" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="O16" s="2">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="P16" s="3">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="R16" s="5">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="S16" s="7">
+        <v>0.97</v>
+      </c>
+      <c r="T16" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="U16" s="3">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="V16" s="3">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="W16" s="5">
+        <v>0.46400000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="1">
+        <v>13</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1.06</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="G17" s="9">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1.01</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="L17" s="8">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="M17" s="10">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="N17" s="2">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="O17" s="2">
+        <v>1.02</v>
+      </c>
+      <c r="P17" s="3">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="R17" s="5">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="S17" s="2">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="T17" s="2">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="U17" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="V17" s="3">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="W17" s="5">
+        <v>0.29699999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="1">
+        <v>13</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1.08</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="F18" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G18" s="3">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="H18" s="5">
+        <v>7.8E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="K18" s="9">
+        <v>0.12</v>
+      </c>
+      <c r="L18" s="3">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="M18" s="5">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="N18" s="2">
+        <v>1.08</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="P18" s="3">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>0.121</v>
+      </c>
+      <c r="R18" s="10">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="S18" s="7">
+        <v>1</v>
+      </c>
+      <c r="T18" s="7">
+        <v>0.84</v>
+      </c>
+      <c r="U18" s="8">
+        <v>0.123</v>
+      </c>
+      <c r="V18" s="3">
+        <v>1.6E-2</v>
+      </c>
+      <c r="W18" s="5">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="1">
+        <v>13</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.76</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="M19" s="5">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="N19" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="P19" s="3">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="R19" s="5">
+        <v>0.59</v>
+      </c>
+      <c r="S19" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="T19" s="7">
+        <v>0.51</v>
+      </c>
+      <c r="U19" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="V19" s="8">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="W19" s="5">
+        <v>0.71799999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="1">
+        <v>12</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1.44</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.33</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="I20" s="2">
+        <v>1.57</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1.51</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="M20" s="5">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="N20" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="O20" s="2">
+        <v>1.51</v>
+      </c>
+      <c r="P20" s="3">
+        <v>0.86</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="R20" s="5">
+        <v>0.504</v>
+      </c>
+      <c r="S20" s="7">
+        <v>1.43</v>
+      </c>
+      <c r="T20" s="7">
+        <v>1.31</v>
+      </c>
+      <c r="U20" s="8">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="V20" s="3">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="W20" s="5">
+        <v>0.53400000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="1">
+        <v>12</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1.06</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="M21" s="5">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="N21" s="7">
+        <v>0.87</v>
+      </c>
+      <c r="O21" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="P21" s="3">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="R21" s="5">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="S21" s="7">
+        <v>0.87</v>
+      </c>
+      <c r="T21" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="U21" s="3">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="V21" s="3">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="W21" s="5">
+        <v>0.41199999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="1">
+        <v>11</v>
+      </c>
+      <c r="D22" s="7">
+        <v>1.18</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.435</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0.215</v>
+      </c>
+      <c r="H22" s="10">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1.28</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1.35</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="L22" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="M22" s="5">
+        <v>0.13</v>
+      </c>
+      <c r="N22" s="2">
+        <v>1.35</v>
+      </c>
+      <c r="O22" s="2">
+        <v>1.36</v>
+      </c>
+      <c r="P22" s="3">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>0.215</v>
+      </c>
+      <c r="R22" s="5">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="S22" s="2">
+        <v>1.36</v>
+      </c>
+      <c r="T22" s="7">
+        <v>1.27</v>
+      </c>
+      <c r="U22" s="8">
+        <v>0.48</v>
+      </c>
+      <c r="V22" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="W22" s="10">
+        <v>0.20399999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="1">
+        <v>10</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1.67</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1.63</v>
+      </c>
+      <c r="F23" s="3">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0.248</v>
+      </c>
+      <c r="H23" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="I23" s="7">
+        <v>1.65</v>
+      </c>
+      <c r="J23" s="7">
+        <v>1.62</v>
+      </c>
+      <c r="K23" s="8">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0.188</v>
+      </c>
+      <c r="M23" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="N23" s="2">
+        <v>1.73</v>
+      </c>
+      <c r="O23" s="7">
+        <v>1.62</v>
+      </c>
+      <c r="P23" s="3">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="R23" s="5">
+        <v>0.111</v>
+      </c>
+      <c r="S23" s="2">
+        <v>1.83</v>
+      </c>
+      <c r="T23" s="2">
+        <v>1.63</v>
+      </c>
+      <c r="U23" s="3">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="V23" s="3">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="W23" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="1">
+        <v>10</v>
+      </c>
+      <c r="D24" s="2">
+        <v>2.13</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1.99</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="I24" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1.89</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="L24" s="3">
+        <v>0.37</v>
+      </c>
+      <c r="M24" s="5">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="N24" s="2">
+        <v>1.82</v>
+      </c>
+      <c r="O24" s="2">
+        <v>1.76</v>
+      </c>
+      <c r="P24" s="3">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="R24" s="5">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="S24" s="7">
+        <v>1.77</v>
+      </c>
+      <c r="T24" s="7">
+        <v>1.54</v>
+      </c>
+      <c r="U24" s="8">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="V24" s="8">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="W24" s="10">
+        <v>0.51100000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="1">
+        <v>10</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1.71</v>
+      </c>
+      <c r="E25" s="7">
+        <v>1.87</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0.188</v>
+      </c>
+      <c r="H25" s="10">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="I25" s="2">
+        <v>1.78</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1.94</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="L25" s="8">
+        <v>0.188</v>
+      </c>
+      <c r="M25" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="N25" s="2">
+        <v>1.81</v>
+      </c>
+      <c r="O25" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="P25" s="3">
+        <v>0.183</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="R25" s="5">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="S25" s="2">
+        <v>1.91</v>
+      </c>
+      <c r="T25" s="2">
+        <v>1.99</v>
+      </c>
+      <c r="U25" s="3">
+        <v>7.8E-2</v>
+      </c>
+      <c r="V25" s="3">
+        <v>-0.03</v>
+      </c>
+      <c r="W25" s="5">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="1">
+        <v>386</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1.73</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1.71</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1.61</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="L26" s="3">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="M26" s="5">
+        <v>0.42</v>
+      </c>
+      <c r="N26" s="2">
+        <v>1.58</v>
+      </c>
+      <c r="O26" s="2">
+        <v>1.56</v>
+      </c>
+      <c r="P26" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="R26" s="5">
+        <v>0.435</v>
+      </c>
+      <c r="S26" s="7">
+        <v>1.54</v>
+      </c>
+      <c r="T26" s="7">
+        <v>1.53</v>
+      </c>
+      <c r="U26" s="8">
+        <v>0.63</v>
+      </c>
+      <c r="V26" s="8">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="W26" s="10">
+        <v>0.44800000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="1">
+        <v>340</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1.64</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1.64</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.495</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1.64</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1.63</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="L27" s="3">
+        <v>0.505</v>
+      </c>
+      <c r="M27" s="5">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="N27" s="2">
+        <v>1.55</v>
+      </c>
+      <c r="O27" s="2">
+        <v>1.55</v>
+      </c>
+      <c r="P27" s="3">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="R27" s="5">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="S27" s="7">
+        <v>1.51</v>
+      </c>
+      <c r="T27" s="7">
+        <v>1.52</v>
+      </c>
+      <c r="U27" s="8">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="V27" s="8">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="W27" s="10">
+        <v>0.41899999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="1">
+        <v>321</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1.76</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1.74</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1.81</v>
+      </c>
+      <c r="J28" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="M28" s="5">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="N28" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="O28" s="2">
+        <v>1.68</v>
+      </c>
+      <c r="P28" s="3">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="R28" s="5">
+        <v>0.33</v>
+      </c>
+      <c r="S28" s="7">
+        <v>1.67</v>
+      </c>
+      <c r="T28" s="7">
+        <v>1.65</v>
+      </c>
+      <c r="U28" s="8">
+        <v>0.503</v>
+      </c>
+      <c r="V28" s="8">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="W28" s="10">
+        <v>0.35899999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="2">
+        <f t="shared" ref="D29:W29" si="0">AVERAGE(D3:D28)</f>
+        <v>1.3473076923076921</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2373076923076924</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="0"/>
+        <v>0.49292307692307691</v>
+      </c>
+      <c r="G29" s="3">
+        <f t="shared" si="0"/>
+        <v>0.4703461538461538</v>
+      </c>
+      <c r="H29" s="8">
+        <f t="shared" si="0"/>
+        <v>0.35780769230769227</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3815384615384618</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2692307692307696</v>
+      </c>
+      <c r="K29" s="3">
+        <f t="shared" si="0"/>
+        <v>0.46526923076923082</v>
+      </c>
+      <c r="L29" s="3">
+        <f t="shared" si="0"/>
+        <v>0.41357692307692318</v>
+      </c>
+      <c r="M29" s="3">
+        <f t="shared" si="0"/>
+        <v>0.30138461538461536</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3665384615384613</v>
+      </c>
+      <c r="O29" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2265384615384618</v>
+      </c>
+      <c r="P29" s="3">
+        <f t="shared" si="0"/>
+        <v>0.51449999999999996</v>
+      </c>
+      <c r="Q29" s="3">
+        <f t="shared" si="0"/>
+        <v>0.45023076923076921</v>
+      </c>
+      <c r="R29" s="3">
+        <f t="shared" si="0"/>
+        <v>0.3297692307692307</v>
+      </c>
+      <c r="S29" s="7">
+        <f t="shared" si="0"/>
+        <v>1.331923076923077</v>
+      </c>
+      <c r="T29" s="7">
+        <f t="shared" si="0"/>
+        <v>1.18</v>
+      </c>
+      <c r="U29" s="8">
+        <f t="shared" si="0"/>
+        <v>0.54461538461538461</v>
+      </c>
+      <c r="V29" s="8">
+        <f t="shared" si="0"/>
+        <v>0.47869230769230781</v>
+      </c>
+      <c r="W29" s="9">
+        <f t="shared" si="0"/>
+        <v>0.35673076923076924</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="2">
+        <f>_xlfn.STDEV.P(D3:D28)</f>
+        <v>0.41388922423859831</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" ref="E30:W30" si="1">_xlfn.STDEV.P(E3:E28)</f>
+        <v>0.37588416477080228</v>
+      </c>
+      <c r="F30" s="3">
+        <f t="shared" si="1"/>
+        <v>0.2163010585480204</v>
+      </c>
+      <c r="G30" s="3">
+        <f t="shared" si="1"/>
+        <v>0.2170331315203162</v>
+      </c>
+      <c r="H30" s="3">
+        <f t="shared" si="1"/>
+        <v>0.1731255700864304</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="1"/>
+        <v>0.3829610575471506</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="1"/>
+        <v>0.36913540435125125</v>
+      </c>
+      <c r="K30" s="3">
+        <f t="shared" si="1"/>
+        <v>0.20940291631433103</v>
+      </c>
+      <c r="L30" s="3">
+        <f t="shared" si="1"/>
+        <v>0.21238303080789644</v>
+      </c>
+      <c r="M30" s="3">
+        <f t="shared" si="1"/>
+        <v>0.16291056463902501</v>
+      </c>
+      <c r="N30" s="2">
+        <f t="shared" si="1"/>
+        <v>0.39488988053820806</v>
+      </c>
+      <c r="O30" s="2">
+        <f t="shared" si="1"/>
+        <v>0.36355025372326222</v>
+      </c>
+      <c r="P30" s="3">
+        <f t="shared" si="1"/>
+        <v>0.21125654291187515</v>
+      </c>
+      <c r="Q30" s="3">
+        <f t="shared" si="1"/>
+        <v>0.21141907120370912</v>
+      </c>
+      <c r="R30" s="3">
+        <f t="shared" si="1"/>
+        <v>0.15822557113484165</v>
+      </c>
+      <c r="S30" s="2">
+        <f t="shared" si="1"/>
+        <v>0.39007907709915934</v>
+      </c>
+      <c r="T30" s="2">
+        <f t="shared" si="1"/>
+        <v>0.3539991308116236</v>
+      </c>
+      <c r="U30" s="3">
+        <f t="shared" si="1"/>
+        <v>0.22803982056499178</v>
+      </c>
+      <c r="V30" s="3">
+        <f t="shared" si="1"/>
+        <v>0.25053953614469215</v>
+      </c>
+      <c r="W30" s="3">
+        <f t="shared" si="1"/>
+        <v>0.18448838981445786</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="I1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>